<commit_message>
Added plist key for status text allignment
</commit_message>
<xml_diff>
--- a/resources/plistPreferenceKeys.xlsx
+++ b/resources/plistPreferenceKeys.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/Downloads/DEPNotify 2018-11-03 14-13-22 - fgd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/GitHub/DEP-Notify/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{E409D45C-8B0E-194F-BB66-48E15F9DD297}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{C30E68E0-300D-0F4B-AD84-04FCE2984449}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="460" windowWidth="28020" windowHeight="16060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="177">
   <si>
     <t>Domain</t>
   </si>
@@ -549,6 +549,18 @@
   </si>
   <si>
     <t>textField1Bubble</t>
+  </si>
+  <si>
+    <t>Main Screen Status Text</t>
+  </si>
+  <si>
+    <t>statusTextAlignment</t>
+  </si>
+  <si>
+    <t>Sets the main screen status text alignment under the progress bar</t>
+  </si>
+  <si>
+    <t>statusTextAlignment left (options are left, center, or right)</t>
   </si>
 </sst>
 </file>
@@ -689,7 +701,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{DF359792-DFC7-9149-8E73-A00A99146929}" diskRevisions="1" revisionId="205" version="5">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{3DE35F53-B5EC-CB47-8D76-2F7DA4820820}" diskRevisions="1" revisionId="216" version="6">
   <header guid="{C0798799-DC42-A843-A3E5-6AC56D32C1C2}" dateTime="2018-11-02T18:51:55" maxSheetId="2" userName="Federico Deis" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -714,6 +726,12 @@
     </sheetIdMap>
   </header>
   <header guid="{DF359792-DFC7-9149-8E73-A00A99146929}" dateTime="2018-11-03T17:05:21" maxSheetId="3" userName="Kyle Bareis" r:id="rId5" minRId="195" maxRId="205">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{3DE35F53-B5EC-CB47-8D76-2F7DA4820820}" dateTime="2018-11-03T17:59:41" maxSheetId="3" userName="Kyle Bareis" r:id="rId6" minRId="206" maxRId="216">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -3190,9 +3208,423 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="206" sId="2" ref="A4:XFD4" action="insertRow"/>
+  <rrc rId="207" sId="2" ref="A4:XFD4" action="insertRow"/>
+  <rm rId="208" sheetId="2" source="A6:XFD6" destination="A4:XFD4" sourceSheetId="2">
+    <rfmt sheetId="2" xfDxf="1" sqref="A4:XFD4" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+        </font>
+        <alignment vertical="center"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="A4" start="0" length="0">
+      <dxf>
+        <font>
+          <b/>
+          <sz val="11"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          </patternFill>
+        </fill>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="B4" start="0" length="0">
+      <dxf>
+        <font>
+          <b/>
+          <sz val="11"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          </patternFill>
+        </fill>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="C4" start="0" length="0">
+      <dxf>
+        <font>
+          <b/>
+          <sz val="11"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          </patternFill>
+        </fill>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="D4" start="0" length="0">
+      <dxf>
+        <font>
+          <b/>
+          <sz val="11"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          </patternFill>
+        </fill>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="E4" start="0" length="0">
+      <dxf>
+        <font>
+          <b/>
+          <sz val="11"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          </patternFill>
+        </fill>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="F4" start="0" length="0">
+      <dxf>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          </patternFill>
+        </fill>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rm rId="209" sheetId="2" source="A6:XFD6" destination="A5:XFD5" sourceSheetId="2">
+    <rfmt sheetId="2" xfDxf="1" sqref="A5:XFD5" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+        </font>
+        <alignment vertical="center"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="A5" start="0" length="0">
+      <dxf>
+        <font>
+          <b/>
+          <sz val="11"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          </patternFill>
+        </fill>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="B5" start="0" length="0">
+      <dxf>
+        <font>
+          <b/>
+          <sz val="11"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          </patternFill>
+        </fill>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="C5" start="0" length="0">
+      <dxf>
+        <font>
+          <b/>
+          <sz val="11"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          </patternFill>
+        </fill>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="D5" start="0" length="0">
+      <dxf>
+        <font>
+          <b/>
+          <sz val="11"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          </patternFill>
+        </fill>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="E5" start="0" length="0">
+      <dxf>
+        <font>
+          <b/>
+          <sz val="11"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          </patternFill>
+        </fill>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="F5" start="0" length="0">
+      <dxf>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          </patternFill>
+        </fill>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rfmt sheetId="2" sqref="A5" start="0" length="0">
+    <dxf>
+      <font>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center"/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" sqref="B5" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center"/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" sqref="C5" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center"/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" sqref="D5" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center"/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" sqref="E5" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center"/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" sqref="F5" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center"/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" sqref="A5:XFD5" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Helvetica"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="210" sId="2">
+    <nc r="A5" t="inlineStr">
+      <is>
+        <t>Main Screen Status Text</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="211" sId="2">
+    <nc r="A6" t="inlineStr">
+      <is>
+        <t>menu.nomad.DEPNotify</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="2" sqref="A6:XFD6" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <sz val="11"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="212" sId="2" xfDxf="1" dxf="1">
+    <nc r="B6" t="inlineStr">
+      <is>
+        <t>statusTextAlignment</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <sz val="11"/>
+      </font>
+    </ndxf>
+  </rcc>
+  <rcc rId="213" sId="2">
+    <nc r="C6" t="inlineStr">
+      <is>
+        <t>String</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="214" sId="2">
+    <nc r="D6" t="inlineStr">
+      <is>
+        <t>Sets the main screen status text alignment under the progress bar</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="215" sId="2">
+    <nc r="E6" t="inlineStr">
+      <is>
+        <t>defaults write menu.nomad.DEPNotify</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="2" xfDxf="1" sqref="F6" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="11"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="216" sId="2">
+    <nc r="F6" t="inlineStr">
+      <is>
+        <t>statusTextAlignment left (options are left, center, or right)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}" action="delete"/>
+  <rcv guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{1878CFB4-398A-014D-AECB-FA656DF31DD8}" name="Federico Deis" id="-2001004240" dateTime="2018-11-03T13:11:43"/>
+  <userInfo guid="{3DE35F53-B5EC-CB47-8D76-2F7DA4820820}" name="Kyle Bareis" id="-368575707" dateTime="2018-11-03T17:55:55"/>
 </users>
 </file>
 
@@ -4039,10 +4471,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E3AB8B7-C63D-3E45-856D-77E679403626}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4100,7 +4532,7 @@
     </row>
     <row r="5" spans="1:6" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>97</v>
+        <v>173</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -4113,109 +4545,99 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" s="5" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="5" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="5" t="s">
+    <row r="9" spans="1:6" s="5" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>148</v>
-      </c>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4223,19 +4645,19 @@
         <v>4</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4243,19 +4665,19 @@
         <v>4</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4263,19 +4685,19 @@
         <v>4</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4283,19 +4705,19 @@
         <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4303,19 +4725,19 @@
         <v>4</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4323,19 +4745,19 @@
         <v>4</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4343,19 +4765,19 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4363,19 +4785,19 @@
         <v>4</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>162</v>
+      <c r="F19" s="5" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4383,19 +4805,19 @@
         <v>4</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>158</v>
+      <c r="F20" s="5" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4403,19 +4825,19 @@
         <v>4</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>159</v>
+      <c r="F21" s="7" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4423,19 +4845,19 @@
         <v>4</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>160</v>
+      <c r="F22" s="7" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4443,99 +4865,99 @@
         <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>172</v>
+      <c r="B24" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>171</v>
+      <c r="B25" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>135</v>
+      <c r="B26" s="14" t="s">
+        <v>172</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>136</v>
+      <c r="B27" s="14" t="s">
+        <v>171</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4543,19 +4965,19 @@
         <v>4</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4563,80 +4985,86 @@
         <v>4</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F29" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
+    <row r="32" spans="1:6" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4644,22 +5072,56 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}" topLeftCell="A11">
-      <selection activeCell="D19" sqref="D19"/>
+    <customSheetView guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}" topLeftCell="B1">
+      <selection activeCell="F6" sqref="F6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{9FC80166-3721-9A4D-A675-78A688924A11}">

</xml_diff>

<commit_message>
Updating all the plist calls
</commit_message>
<xml_diff>
--- a/resources/plistPreferenceKeys.xlsx
+++ b/resources/plistPreferenceKeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/GitHub/DEP-Notify/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{6F14B611-9074-F143-81CE-5CB36BCAE28E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{3CE9CD0A-7840-CB46-BA64-CAEB0E4FA6D3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="460" windowWidth="28020" windowHeight="16060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -701,7 +701,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{9F6066B3-895E-D847-BF13-9E2C20972BC6}" diskRevisions="1" revisionId="216" version="7">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{38DB3D6A-6ECE-6747-A9E8-CD3D0A0096C2}" diskRevisions="1" revisionId="220" version="8">
   <header guid="{C0798799-DC42-A843-A3E5-6AC56D32C1C2}" dateTime="2018-11-02T18:51:55" maxSheetId="2" userName="Federico Deis" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -738,6 +738,12 @@
     </sheetIdMap>
   </header>
   <header guid="{9F6066B3-895E-D847-BF13-9E2C20972BC6}" dateTime="2018-11-03T18:26:23" maxSheetId="3" userName="Kyle Bareis" r:id="rId7">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{38DB3D6A-6ECE-6747-A9E8-CD3D0A0096C2}" dateTime="2018-11-03T20:52:46" maxSheetId="3" userName="Kyle Bareis" r:id="rId8" minRId="217" maxRId="220">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -3634,9 +3640,160 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="217" sId="2" ref="A18:XFD19" action="insertRow"/>
+  <rm rId="218" sheetId="2" source="A28:XFD29" destination="A18:XFD19" sourceSheetId="2">
+    <rfmt sheetId="2" xfDxf="1" sqref="A18:XFD18" start="0" length="0"/>
+    <rfmt sheetId="2" xfDxf="1" sqref="A19:XFD19" start="0" length="0"/>
+    <rfmt sheetId="2" sqref="A18" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Helvetica"/>
+          <family val="2"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="B18" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Helvetica"/>
+          <family val="2"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="C18" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Helvetica"/>
+          <family val="2"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="D18" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Helvetica"/>
+          <family val="2"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="E18" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Helvetica"/>
+          <family val="2"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="F18" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Helvetica"/>
+          <family val="2"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="A19" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Helvetica"/>
+          <family val="2"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="B19" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Helvetica"/>
+          <family val="2"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="C19" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Helvetica"/>
+          <family val="2"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="D19" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Helvetica"/>
+          <family val="2"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="E19" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Helvetica"/>
+          <family val="2"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="F19" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Helvetica"/>
+          <family val="2"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+  </rm>
+  <rrc rId="219" sId="2" ref="A28:XFD28" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A28:XFD28" start="0" length="0"/>
+  </rrc>
+  <rrc rId="220" sId="2" ref="A28:XFD28" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A28:XFD28" start="0" length="0"/>
+  </rrc>
+  <rcv guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}" action="delete"/>
+  <rcv guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{1878CFB4-398A-014D-AECB-FA656DF31DD8}" name="Federico Deis" id="-2001004240" dateTime="2018-11-03T13:11:43"/>
+  <userInfo guid="{38DB3D6A-6ECE-6747-A9E8-CD3D0A0096C2}" name="Kyle Bareis" id="-368587326" dateTime="2018-11-03T19:37:42"/>
 </users>
 </file>
 
@@ -4485,8 +4642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E3AB8B7-C63D-3E45-856D-77E679403626}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4776,40 +4933,40 @@
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>113</v>
+      <c r="B18" s="14" t="s">
+        <v>172</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>115</v>
+      <c r="B19" s="14" t="s">
+        <v>171</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4817,19 +4974,19 @@
         <v>4</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4837,19 +4994,19 @@
         <v>4</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>162</v>
+      <c r="F21" s="5" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4857,19 +5014,19 @@
         <v>4</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>158</v>
+      <c r="F22" s="5" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4877,19 +5034,19 @@
         <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>159</v>
+      <c r="F23" s="7" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4897,19 +5054,19 @@
         <v>4</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>160</v>
+      <c r="F24" s="7" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4917,59 +5074,59 @@
         <v>4</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="14" t="s">
-        <v>172</v>
+      <c r="B26" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>171</v>
+      <c r="B27" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>143</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5132,8 +5289,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}">
-      <selection activeCell="F6" sqref="F6"/>
+    <customSheetView guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}" topLeftCell="A13">
+      <selection activeCell="A21" sqref="A21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{9FC80166-3721-9A4D-A675-78A688924A11}">

</xml_diff>

<commit_message>
Finished rough additions. Needs more debugging
</commit_message>
<xml_diff>
--- a/resources/plistPreferenceKeys.xlsx
+++ b/resources/plistPreferenceKeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/GitHub/DEP-Notify/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{3CE9CD0A-7840-CB46-BA64-CAEB0E4FA6D3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{62D6A7ED-2D75-2D4C-9985-9B1A6509349F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="460" windowWidth="28020" windowHeight="16060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3790,10 +3790,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
   <userInfo guid="{1878CFB4-398A-014D-AECB-FA656DF31DD8}" name="Federico Deis" id="-2001004240" dateTime="2018-11-03T13:11:43"/>
-  <userInfo guid="{38DB3D6A-6ECE-6747-A9E8-CD3D0A0096C2}" name="Kyle Bareis" id="-368587326" dateTime="2018-11-03T19:37:42"/>
 </users>
 </file>
 
@@ -4642,8 +4641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E3AB8B7-C63D-3E45-856D-77E679403626}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fgd depluralized a few keys
changed contents to content and uploaded new spreadsheet
</commit_message>
<xml_diff>
--- a/resources/plistPreferenceKeys.xlsx
+++ b/resources/plistPreferenceKeys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/GitHub/DEP-Notify/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{223D1E04-A00C-3049-B1EC-DA52D47CFE16}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{BF935AE4-BADE-FA4F-87DC-5414B5F0ED0F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="460" windowWidth="28020" windowHeight="16060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,18 +395,6 @@
     <t>Enables popup button 4 and sets custom label</t>
   </si>
   <si>
-    <t>popupButton1Contents</t>
-  </si>
-  <si>
-    <t>popupButton2Contents</t>
-  </si>
-  <si>
-    <t>popupButton3Contents</t>
-  </si>
-  <si>
-    <t>popupButton4Contents</t>
-  </si>
-  <si>
     <t>Contents of the popup menu 1</t>
   </si>
   <si>
@@ -485,9 +473,6 @@
     <t xml:space="preserve"> pathToPlistFile "/My/Path/myplistfile.plist</t>
   </si>
   <si>
-    <t>textField2sOptional -bool false or 0</t>
-  </si>
-  <si>
     <t>textFieldIsOptional -bool true or 1</t>
   </si>
   <si>
@@ -497,24 +482,12 @@
     <t>popupButton1Label "Computer Type"</t>
   </si>
   <si>
-    <t>popupButton1Contents -array "US" "APAC" "Europe" "Americas"</t>
-  </si>
-  <si>
-    <t>popupButton2Contents -array "Primary" "Secondary" "Shared"</t>
-  </si>
-  <si>
-    <t>popupButton3Contents -array "Corporate Owned" "BYOD" "Third Party Provided"</t>
-  </si>
-  <si>
     <t>popupButton2Label "Asset Owner"</t>
   </si>
   <si>
     <t>popupButton3Label "User Type"</t>
   </si>
   <si>
-    <t>popupButton4Contents -array "Standard" "Privileged" "Temoporary"</t>
-  </si>
-  <si>
     <t>textFIeld1Bubble -array "Title" "Informative text"</t>
   </si>
   <si>
@@ -579,6 +552,33 @@
   </si>
   <si>
     <t>helpBubbleBody "Here is how can I help you"</t>
+  </si>
+  <si>
+    <t>popupButton1Content</t>
+  </si>
+  <si>
+    <t>popupButton2Content</t>
+  </si>
+  <si>
+    <t>popupButton3Content</t>
+  </si>
+  <si>
+    <t>popupButton4Content</t>
+  </si>
+  <si>
+    <t>popupButton1Content -array "US" "APAC" "Europe" "Americas"</t>
+  </si>
+  <si>
+    <t>popupButton2Content -array "Primary" "Secondary" "Shared"</t>
+  </si>
+  <si>
+    <t>popupButton3Content -array "Corporate Owned" "BYOD" "Third Party Provided"</t>
+  </si>
+  <si>
+    <t>popupButton4Content -array "Standard" "Privileged" "Temoporary"</t>
+  </si>
+  <si>
+    <t>textField2IsOptional -bool false or 0</t>
   </si>
 </sst>
 </file>
@@ -722,7 +722,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B6FA5F59-A05A-924E-93D0-47E016FDB805}" diskRevisions="1" revisionId="238" version="13">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A120FAA6-2724-774E-A65F-3797652A47D1}" diskRevisions="1" revisionId="247" version="15">
   <header guid="{C0798799-DC42-A843-A3E5-6AC56D32C1C2}" dateTime="2018-11-02T18:51:55" maxSheetId="2" userName="Federico Deis" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -800,6 +800,18 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{A1722660-1D8B-4045-A8AC-05A5E68EB82B}" dateTime="2018-11-19T12:15:08" maxSheetId="3" userName="Kyle Bareis" r:id="rId14" minRId="239" maxRId="246">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A120FAA6-2724-774E-A65F-3797652A47D1}" dateTime="2018-11-19T12:15:56" maxSheetId="3" userName="Kyle Bareis" r:id="rId15" minRId="247">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -886,6 +898,126 @@
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}" action="delete"/>
   <rcv guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="239" sId="2">
+    <oc r="B26" t="inlineStr">
+      <is>
+        <t>popupButton1Contents</t>
+      </is>
+    </oc>
+    <nc r="B26" t="inlineStr">
+      <is>
+        <t>popupButton1Content</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="240" sId="2">
+    <oc r="B27" t="inlineStr">
+      <is>
+        <t>popupButton2Contents</t>
+      </is>
+    </oc>
+    <nc r="B27" t="inlineStr">
+      <is>
+        <t>popupButton2Content</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="241" sId="2">
+    <oc r="B28" t="inlineStr">
+      <is>
+        <t>popupButton3Contents</t>
+      </is>
+    </oc>
+    <nc r="B28" t="inlineStr">
+      <is>
+        <t>popupButton3Content</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="242" sId="2">
+    <oc r="B29" t="inlineStr">
+      <is>
+        <t>popupButton4Contents</t>
+      </is>
+    </oc>
+    <nc r="B29" t="inlineStr">
+      <is>
+        <t>popupButton4Content</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="243" sId="2">
+    <oc r="F26" t="inlineStr">
+      <is>
+        <t>popupButton1Contents -array "US" "APAC" "Europe" "Americas"</t>
+      </is>
+    </oc>
+    <nc r="F26" t="inlineStr">
+      <is>
+        <t>popupButton1Content -array "US" "APAC" "Europe" "Americas"</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="244" sId="2">
+    <oc r="F27" t="inlineStr">
+      <is>
+        <t>popupButton2Contents -array "Primary" "Secondary" "Shared"</t>
+      </is>
+    </oc>
+    <nc r="F27" t="inlineStr">
+      <is>
+        <t>popupButton2Content -array "Primary" "Secondary" "Shared"</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="245" sId="2">
+    <oc r="F28" t="inlineStr">
+      <is>
+        <t>popupButton3Contents -array "Corporate Owned" "BYOD" "Third Party Provided"</t>
+      </is>
+    </oc>
+    <nc r="F28" t="inlineStr">
+      <is>
+        <t>popupButton3Content -array "Corporate Owned" "BYOD" "Third Party Provided"</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="246" sId="2">
+    <oc r="F29" t="inlineStr">
+      <is>
+        <t>popupButton4Contents -array "Standard" "Privileged" "Temoporary"</t>
+      </is>
+    </oc>
+    <nc r="F29" t="inlineStr">
+      <is>
+        <t>popupButton4Content -array "Standard" "Privileged" "Temoporary"</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}" action="delete"/>
+  <rcv guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="247" sId="2">
+    <oc r="F19" t="inlineStr">
+      <is>
+        <t>textField2sOptional -bool false or 0</t>
+      </is>
+    </oc>
+    <nc r="F19" t="inlineStr">
+      <is>
+        <t>textField2IsOptional -bool false or 0</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -5048,8 +5180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E3AB8B7-C63D-3E45-856D-77E679403626}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5099,15 +5231,15 @@
         <v>102</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -5120,19 +5252,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5159,10 +5291,10 @@
         <v>98</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="5" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5179,10 +5311,10 @@
         <v>99</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5209,10 +5341,10 @@
         <v>110</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5229,10 +5361,10 @@
         <v>111</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5249,10 +5381,10 @@
         <v>112</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5266,13 +5398,13 @@
         <v>6</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5286,13 +5418,13 @@
         <v>6</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="5" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5300,19 +5432,19 @@
         <v>4</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5320,19 +5452,19 @@
         <v>4</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5346,13 +5478,13 @@
         <v>46</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5366,13 +5498,13 @@
         <v>46</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>151</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5380,19 +5512,19 @@
         <v>4</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5400,19 +5532,19 @@
         <v>4</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5429,10 +5561,10 @@
         <v>114</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5449,10 +5581,10 @@
         <v>118</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5469,10 +5601,10 @@
         <v>119</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5489,10 +5621,10 @@
         <v>120</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5500,19 +5632,19 @@
         <v>4</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5520,19 +5652,19 @@
         <v>4</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>122</v>
+        <v>175</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5540,19 +5672,19 @@
         <v>4</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5560,19 +5692,19 @@
         <v>4</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>124</v>
+        <v>177</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5580,19 +5712,19 @@
         <v>4</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>143</v>
-      </c>
       <c r="F30" s="5" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5600,19 +5732,19 @@
         <v>4</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5620,19 +5752,19 @@
         <v>4</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -5640,24 +5772,24 @@
         <v>4</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -5735,8 +5867,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}">
-      <selection activeCell="F4" sqref="F4"/>
+    <customSheetView guid="{9EC86DF9-1CFA-EB43-BA3E-6F36FBBDD43C}" topLeftCell="B22">
+      <selection activeCell="F30" sqref="F30"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{9FC80166-3721-9A4D-A675-78A688924A11}">

</xml_diff>